<commit_message>
this version is working
</commit_message>
<xml_diff>
--- a/ExcelExample.xlsx
+++ b/ExcelExample.xlsx
@@ -12,39 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Datatype</t>
+    <t>Email</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>Size(in bytes)</t>
+    <t>postcode</t>
   </si>
   <si>
-    <t>int</t>
+    <t>peter.krawiec@qa.com</t>
   </si>
   <si>
-    <t>Primitive</t>
+    <t>Password1</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>char</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Non-Primitive</t>
-  </si>
-  <si>
-    <t>No fixed size</t>
+    <t>M50 2BB</t>
   </si>
 </sst>
 </file>
@@ -113,52 +98,8 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>